<commit_message>
se actualiza el diccionario de datos
</commit_message>
<xml_diff>
--- a/public/AUXILIAR CON SALDOS 20210131.xlsx
+++ b/public/AUXILIAR CON SALDOS 20210131.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FABIOROJAS\Downloads\yopal-testing\examples-dicc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.rojas\code\produccion\csv-analyzer\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F66382C-AC64-4C38-953A-94429CDA8120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCA85E5-9481-4105-8CCC-3CA8BCD89089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85A88BE5-FA58-4E42-816D-109A4E858F8A}"/>
+    <workbookView xWindow="9180" yWindow="2184" windowWidth="15912" windowHeight="8172" xr2:uid="{85A88BE5-FA58-4E42-816D-109A4E858F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Anio</t>
   </si>
@@ -63,15 +54,9 @@
     <t>Centro_Costos</t>
   </si>
   <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
     <t>Tercero</t>
   </si>
   <si>
-    <t>Identificacion</t>
-  </si>
-  <si>
     <t>Codigo_Contable</t>
   </si>
   <si>
@@ -81,18 +66,9 @@
     <t>Creditos</t>
   </si>
   <si>
-    <t>Saldo_Total_Debito</t>
-  </si>
-  <si>
-    <t>Saldo_Total_Credito</t>
-  </si>
-  <si>
     <t>Macro_campo_nivel_agregado</t>
   </si>
   <si>
-    <t>Saldo_Inicial</t>
-  </si>
-  <si>
     <t>Alcaldia del Municipio A</t>
   </si>
   <si>
@@ -112,6 +88,15 @@
   </si>
   <si>
     <t>DA</t>
+  </si>
+  <si>
+    <t>Descripcion_Registro_Contable</t>
+  </si>
+  <si>
+    <t>Identificacion_Tercero</t>
+  </si>
+  <si>
+    <t>Descripcion_codigo_contable</t>
   </si>
 </sst>
 </file>
@@ -516,30 +501,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4231599-D038-4DD2-B2B1-013225DD506D}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" customWidth="1"/>
-    <col min="13" max="13" width="25.28515625" customWidth="1"/>
-    <col min="17" max="17" width="22" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" customWidth="1"/>
-    <col min="19" max="19" width="34.5703125" customWidth="1"/>
-    <col min="20" max="20" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="31.44140625" customWidth="1"/>
+    <col min="12" max="12" width="22.44140625" customWidth="1"/>
+    <col min="13" max="13" width="25.33203125" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" customWidth="1"/>
+    <col min="17" max="17" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -568,40 +552,31 @@
         <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2018</v>
       </c>
@@ -609,25 +584,25 @@
         <v>900900081</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3">
         <v>201800513</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L2" s="2">
         <v>900900081</v>
@@ -636,7 +611,7 @@
         <v>615560</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O2" s="2">
         <v>1000000.35</v>
@@ -644,17 +619,8 @@
       <c r="P2" s="2">
         <v>1000000.35</v>
       </c>
-      <c r="Q2" s="2">
-        <v>29000000.280000001</v>
-      </c>
-      <c r="R2" s="2">
-        <v>19000000.41</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" s="2">
-        <v>19000000.41</v>
+      <c r="Q2" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>